<commit_message>
Update supplementary files with published files
</commit_message>
<xml_diff>
--- a/Additional_file_1.xlsx
+++ b/Additional_file_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thordis\Documents\GitHub\Lbreuteri\Article\Supplementary_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A45F5EB-B8A4-4386-937A-CEF78D1870C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58708886-29E9-4E15-8476-C0C80CDC5725}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="6225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="6225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset for energy req." sheetId="1" r:id="rId1"/>
@@ -874,16 +874,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -894,6 +884,16 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -10341,7 +10341,7 @@
   </sheetPr>
   <dimension ref="A1:AJ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -12180,8 +12180,8 @@
   </sheetPr>
   <dimension ref="A1:AJ963"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I90" sqref="I90"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -12201,7 +12201,7 @@
     </row>
     <row r="3" spans="1:36" s="2" customFormat="1"/>
     <row r="4" spans="1:36">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="137" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="126"/>
@@ -12311,7 +12311,7 @@
       <c r="AJ5" s="4"/>
     </row>
     <row r="6" spans="1:36">
-      <c r="A6" s="133" t="s">
+      <c r="A6" s="138" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="108">
@@ -12381,7 +12381,7 @@
       <c r="AJ6" s="4"/>
     </row>
     <row r="7" spans="1:36">
-      <c r="A7" s="134"/>
+      <c r="A7" s="139"/>
       <c r="B7" s="108">
         <v>1</v>
       </c>
@@ -12449,7 +12449,7 @@
       <c r="AJ7" s="4"/>
     </row>
     <row r="8" spans="1:36">
-      <c r="A8" s="134"/>
+      <c r="A8" s="139"/>
       <c r="B8" s="108">
         <v>1</v>
       </c>
@@ -12517,7 +12517,7 @@
       <c r="AJ8" s="4"/>
     </row>
     <row r="9" spans="1:36">
-      <c r="A9" s="134"/>
+      <c r="A9" s="139"/>
       <c r="B9" s="108">
         <v>1</v>
       </c>
@@ -12585,7 +12585,7 @@
       <c r="AJ9" s="4"/>
     </row>
     <row r="10" spans="1:36">
-      <c r="A10" s="134"/>
+      <c r="A10" s="139"/>
       <c r="B10" s="108">
         <v>1</v>
       </c>
@@ -12653,7 +12653,7 @@
       <c r="AJ10" s="4"/>
     </row>
     <row r="11" spans="1:36">
-      <c r="A11" s="134"/>
+      <c r="A11" s="139"/>
       <c r="B11" s="108">
         <v>1</v>
       </c>
@@ -12721,7 +12721,7 @@
       <c r="AJ11" s="4"/>
     </row>
     <row r="12" spans="1:36">
-      <c r="A12" s="134"/>
+      <c r="A12" s="139"/>
       <c r="B12" s="108">
         <v>1</v>
       </c>
@@ -12789,7 +12789,7 @@
       <c r="AJ12" s="4"/>
     </row>
     <row r="13" spans="1:36">
-      <c r="A13" s="134"/>
+      <c r="A13" s="139"/>
       <c r="B13" s="109">
         <v>2</v>
       </c>
@@ -12855,7 +12855,7 @@
       <c r="AJ13" s="4"/>
     </row>
     <row r="14" spans="1:36">
-      <c r="A14" s="134"/>
+      <c r="A14" s="139"/>
       <c r="B14" s="109">
         <v>2</v>
       </c>
@@ -12921,7 +12921,7 @@
       <c r="AJ14" s="4"/>
     </row>
     <row r="15" spans="1:36">
-      <c r="A15" s="134"/>
+      <c r="A15" s="139"/>
       <c r="B15" s="109">
         <v>2</v>
       </c>
@@ -12987,7 +12987,7 @@
       <c r="AJ15" s="4"/>
     </row>
     <row r="16" spans="1:36">
-      <c r="A16" s="134"/>
+      <c r="A16" s="139"/>
       <c r="B16" s="109">
         <v>2</v>
       </c>
@@ -13053,7 +13053,7 @@
       <c r="AJ16" s="4"/>
     </row>
     <row r="17" spans="1:36">
-      <c r="A17" s="134"/>
+      <c r="A17" s="139"/>
       <c r="B17" s="109">
         <v>2</v>
       </c>
@@ -13111,7 +13111,7 @@
       <c r="AJ17" s="4"/>
     </row>
     <row r="18" spans="1:36">
-      <c r="A18" s="134"/>
+      <c r="A18" s="139"/>
       <c r="B18" s="109">
         <v>2</v>
       </c>
@@ -13169,7 +13169,7 @@
       <c r="AJ18" s="4"/>
     </row>
     <row r="19" spans="1:36">
-      <c r="A19" s="134"/>
+      <c r="A19" s="139"/>
       <c r="B19" s="110">
         <v>3</v>
       </c>
@@ -13235,7 +13235,7 @@
       <c r="AJ19" s="4"/>
     </row>
     <row r="20" spans="1:36">
-      <c r="A20" s="134"/>
+      <c r="A20" s="139"/>
       <c r="B20" s="110">
         <v>3</v>
       </c>
@@ -13301,7 +13301,7 @@
       <c r="AJ20" s="4"/>
     </row>
     <row r="21" spans="1:36">
-      <c r="A21" s="134"/>
+      <c r="A21" s="139"/>
       <c r="B21" s="110">
         <v>3</v>
       </c>
@@ -13367,7 +13367,7 @@
       <c r="AJ21" s="4"/>
     </row>
     <row r="22" spans="1:36">
-      <c r="A22" s="134"/>
+      <c r="A22" s="139"/>
       <c r="B22" s="110">
         <v>3</v>
       </c>
@@ -13433,7 +13433,7 @@
       <c r="AJ22" s="4"/>
     </row>
     <row r="23" spans="1:36">
-      <c r="A23" s="134"/>
+      <c r="A23" s="139"/>
       <c r="B23" s="110">
         <v>3</v>
       </c>
@@ -13491,7 +13491,7 @@
       <c r="AJ23" s="4"/>
     </row>
     <row r="24" spans="1:36">
-      <c r="A24" s="134"/>
+      <c r="A24" s="139"/>
       <c r="B24" s="110">
         <v>3</v>
       </c>
@@ -13549,7 +13549,7 @@
       <c r="AJ24" s="4"/>
     </row>
     <row r="25" spans="1:36">
-      <c r="A25" s="133" t="s">
+      <c r="A25" s="138" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="109">
@@ -13617,7 +13617,7 @@
       <c r="AJ25" s="4"/>
     </row>
     <row r="26" spans="1:36">
-      <c r="A26" s="134"/>
+      <c r="A26" s="139"/>
       <c r="B26" s="109">
         <v>1</v>
       </c>
@@ -13683,7 +13683,7 @@
       <c r="AJ26" s="4"/>
     </row>
     <row r="27" spans="1:36">
-      <c r="A27" s="134"/>
+      <c r="A27" s="139"/>
       <c r="B27" s="109">
         <v>1</v>
       </c>
@@ -13749,7 +13749,7 @@
       <c r="AJ27" s="4"/>
     </row>
     <row r="28" spans="1:36">
-      <c r="A28" s="134"/>
+      <c r="A28" s="139"/>
       <c r="B28" s="109">
         <v>1</v>
       </c>
@@ -13815,7 +13815,7 @@
       <c r="AJ28" s="4"/>
     </row>
     <row r="29" spans="1:36">
-      <c r="A29" s="134"/>
+      <c r="A29" s="139"/>
       <c r="B29" s="109">
         <v>1</v>
       </c>
@@ -13873,7 +13873,7 @@
       <c r="AJ29" s="4"/>
     </row>
     <row r="30" spans="1:36">
-      <c r="A30" s="134"/>
+      <c r="A30" s="139"/>
       <c r="B30" s="109">
         <v>1</v>
       </c>
@@ -13931,7 +13931,7 @@
       <c r="AJ30" s="4"/>
     </row>
     <row r="31" spans="1:36">
-      <c r="A31" s="134"/>
+      <c r="A31" s="139"/>
       <c r="B31" s="110">
         <v>2</v>
       </c>
@@ -13997,7 +13997,7 @@
       <c r="AJ31" s="4"/>
     </row>
     <row r="32" spans="1:36">
-      <c r="A32" s="134"/>
+      <c r="A32" s="139"/>
       <c r="B32" s="110">
         <v>2</v>
       </c>
@@ -14063,7 +14063,7 @@
       <c r="AJ32" s="4"/>
     </row>
     <row r="33" spans="1:36">
-      <c r="A33" s="134"/>
+      <c r="A33" s="139"/>
       <c r="B33" s="110">
         <v>2</v>
       </c>
@@ -14129,7 +14129,7 @@
       <c r="AJ33" s="4"/>
     </row>
     <row r="34" spans="1:36">
-      <c r="A34" s="134"/>
+      <c r="A34" s="139"/>
       <c r="B34" s="110">
         <v>2</v>
       </c>
@@ -14195,7 +14195,7 @@
       <c r="AJ34" s="4"/>
     </row>
     <row r="35" spans="1:36">
-      <c r="A35" s="134"/>
+      <c r="A35" s="139"/>
       <c r="B35" s="110">
         <v>2</v>
       </c>
@@ -14253,7 +14253,7 @@
       <c r="AJ35" s="4"/>
     </row>
     <row r="36" spans="1:36">
-      <c r="A36" s="134"/>
+      <c r="A36" s="139"/>
       <c r="B36" s="110">
         <v>2</v>
       </c>
@@ -14497,17 +14497,17 @@
       <c r="AJ40" s="4"/>
     </row>
     <row r="41" spans="1:36">
-      <c r="A41" s="135" t="s">
+      <c r="A41" s="136" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="29">
         <v>1</v>
       </c>
       <c r="C41" s="30">
-        <v>0.3833333332751252</v>
+        <v>0.38333333327512498</v>
       </c>
       <c r="D41" s="30">
-        <v>4.9450022727272731E-2</v>
+        <v>4.9450022727272697E-2</v>
       </c>
       <c r="E41" s="30">
         <v>-3.0067927613124552</v>
@@ -14899,7 +14899,7 @@
       <c r="AJ46" s="32"/>
     </row>
     <row r="47" spans="1:36">
-      <c r="A47" s="135" t="s">
+      <c r="A47" s="136" t="s">
         <v>23</v>
       </c>
       <c r="B47" s="49">
@@ -15347,7 +15347,7 @@
       <c r="AJ54" s="4"/>
     </row>
     <row r="55" spans="1:36">
-      <c r="A55" s="136" t="s">
+      <c r="A55" s="132" t="s">
         <v>21</v>
       </c>
       <c r="B55" s="66">
@@ -15355,14 +15355,14 @@
       </c>
       <c r="C55" s="22">
         <f>(LN(D42/D41))/(C42-C41)</f>
-        <v>0.56867756381347112</v>
+        <v>0.56867756381347123</v>
       </c>
       <c r="D55" s="22">
-        <f t="shared" ref="D55:N55" si="0">SLOPE(F41:F42,$D41:$D42)*SLOPE($E41:$E42,$C41:$C42)</f>
+        <f>SLOPE(F41:F42,$D41:$D42)*SLOPE($E41:$E42,$C41:$C42)</f>
         <v>-17.654518064415132</v>
       </c>
       <c r="E55" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D55:N55" si="0">SLOPE(G41:G42,$D41:$D42)*SLOPE($E41:$E42,$C41:$C42)</f>
         <v>0</v>
       </c>
       <c r="F55" s="22">
@@ -15379,7 +15379,7 @@
       </c>
       <c r="I55" s="22">
         <f t="shared" si="0"/>
-        <v>-0.18545184747808438</v>
+        <v>-0.18545184747808441</v>
       </c>
       <c r="J55" s="22">
         <f t="shared" si="0"/>
@@ -15391,11 +15391,11 @@
       </c>
       <c r="L55" s="22">
         <f t="shared" si="0"/>
-        <v>-0.31193302341221829</v>
+        <v>-0.31193302341221835</v>
       </c>
       <c r="M55" s="22">
         <f t="shared" si="0"/>
-        <v>-0.80828800605086393</v>
+        <v>-0.80828800605086404</v>
       </c>
       <c r="N55" s="22">
         <f t="shared" si="0"/>
@@ -15613,7 +15613,7 @@
       </c>
       <c r="L58" s="58">
         <f t="shared" si="5"/>
-        <v>-0.31193302341221829</v>
+        <v>-0.31193302341221835</v>
       </c>
       <c r="M58" s="58">
         <f t="shared" si="5"/>
@@ -15653,7 +15653,7 @@
       </c>
       <c r="C59" s="22">
         <f t="shared" ref="C59:K59" si="6">STDEV(C55:C57)</f>
-        <v>5.4005735092715897E-2</v>
+        <v>5.4005735092715841E-2</v>
       </c>
       <c r="D59" s="22">
         <f t="shared" si="6"/>
@@ -15692,7 +15692,7 @@
       </c>
       <c r="M59" s="22">
         <f t="shared" ref="M59:N59" si="7">STDEV(M55:M57)</f>
-        <v>0.14458182018846319</v>
+        <v>0.14458182018846358</v>
       </c>
       <c r="N59" s="22">
         <f t="shared" si="7"/>
@@ -15722,7 +15722,7 @@
       <c r="AJ59" s="4"/>
     </row>
     <row r="60" spans="1:36">
-      <c r="A60" s="136" t="s">
+      <c r="A60" s="132" t="s">
         <v>23</v>
       </c>
       <c r="B60" s="66">
@@ -16324,13 +16324,13 @@
       <c r="AJ71" s="4"/>
     </row>
     <row r="72" spans="1:36">
-      <c r="A72" s="137" t="s">
+      <c r="A72" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="B72" s="138"/>
-      <c r="C72" s="138"/>
-      <c r="D72" s="138"/>
-      <c r="E72" s="138"/>
+      <c r="B72" s="134"/>
+      <c r="C72" s="134"/>
+      <c r="D72" s="134"/>
+      <c r="E72" s="134"/>
       <c r="F72" s="26"/>
       <c r="G72" s="26"/>
       <c r="H72" s="26"/>
@@ -17068,11 +17068,11 @@
       <c r="AJ88" s="4"/>
     </row>
     <row r="89" spans="1:36">
-      <c r="A89" s="139" t="s">
+      <c r="A89" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="B89" s="139"/>
-      <c r="C89" s="139"/>
+      <c r="B89" s="135"/>
+      <c r="C89" s="135"/>
       <c r="D89" s="26"/>
       <c r="E89" s="26"/>
       <c r="F89" s="26"/>
@@ -50389,17 +50389,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A72:E72"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A47:A50"/>
     <mergeCell ref="A4:P4"/>
     <mergeCell ref="A39:P39"/>
     <mergeCell ref="A53:N53"/>
     <mergeCell ref="A25:A36"/>
     <mergeCell ref="A41:A46"/>
     <mergeCell ref="A6:A24"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="A72:E72"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A47:A50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -54749,7 +54749,7 @@
       <c r="Q94" s="42"/>
     </row>
     <row r="95" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A95" s="136" t="s">
+      <c r="A95" s="132" t="s">
         <v>22</v>
       </c>
       <c r="B95" s="66">
@@ -55036,7 +55036,7 @@
       <c r="Q99" s="42"/>
     </row>
     <row r="100" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A100" s="136" t="s">
+      <c r="A100" s="132" t="s">
         <v>24</v>
       </c>
       <c r="B100" s="66">
@@ -55320,7 +55320,7 @@
       <c r="Q104" s="42"/>
     </row>
     <row r="105" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A105" s="136" t="s">
+      <c r="A105" s="132" t="s">
         <v>26</v>
       </c>
       <c r="B105" s="66">
@@ -55726,34 +55726,34 @@
       <c r="Q115" s="42"/>
     </row>
     <row r="116" spans="1:20" s="117" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A116" s="139" t="s">
+      <c r="A116" s="135" t="s">
         <v>42</v>
       </c>
-      <c r="B116" s="139"/>
-      <c r="C116" s="139"/>
-      <c r="D116" s="139"/>
+      <c r="B116" s="135"/>
+      <c r="C116" s="135"/>
+      <c r="D116" s="135"/>
       <c r="E116" s="112"/>
-      <c r="F116" s="139" t="s">
+      <c r="F116" s="135" t="s">
         <v>43</v>
       </c>
-      <c r="G116" s="139"/>
-      <c r="H116" s="139"/>
-      <c r="I116" s="139"/>
+      <c r="G116" s="135"/>
+      <c r="H116" s="135"/>
+      <c r="I116" s="135"/>
       <c r="J116" s="112"/>
-      <c r="K116" s="139" t="s">
+      <c r="K116" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="L116" s="139"/>
-      <c r="M116" s="139"/>
-      <c r="N116" s="139"/>
-      <c r="O116" s="139"/>
+      <c r="L116" s="135"/>
+      <c r="M116" s="135"/>
+      <c r="N116" s="135"/>
+      <c r="O116" s="135"/>
       <c r="P116" s="112"/>
-      <c r="Q116" s="139" t="s">
+      <c r="Q116" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="R116" s="139"/>
-      <c r="S116" s="139"/>
-      <c r="T116" s="139"/>
+      <c r="R116" s="135"/>
+      <c r="S116" s="135"/>
+      <c r="T116" s="135"/>
     </row>
     <row r="117" spans="1:20" s="117" customFormat="1" ht="15.75" customHeight="1">
       <c r="A117" s="101" t="s">
@@ -71129,6 +71129,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="Q116:T116"/>
+    <mergeCell ref="K116:O116"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A95:A99"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="F116:I116"/>
     <mergeCell ref="A4:Q4"/>
     <mergeCell ref="A60:Q60"/>
     <mergeCell ref="A90:A94"/>
@@ -71141,13 +71148,6 @@
     <mergeCell ref="A32:A44"/>
     <mergeCell ref="A68:A73"/>
     <mergeCell ref="A74:A79"/>
-    <mergeCell ref="Q116:T116"/>
-    <mergeCell ref="K116:O116"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A95:A99"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="F116:I116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>